<commit_message>
Updated pagination logic to fetch pages dynamically. Merged Hypertension changes from Rupali.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/output/SmartScrappers_Team17_Diabetes_To_Add.xlsx
+++ b/src/test/resources/TestData/output/SmartScrappers_Team17_Diabetes_To_Add.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Recipe ID</t>
   </si>
@@ -45,49 +45,6 @@
   </si>
   <si>
     <t>Targeted Morbid Conditions</t>
-  </si>
-  <si>
-    <t>41708</t>
-  </si>
-  <si>
-    <t>quinoa dosa recipe | healthy quinoa dosa | quinoa urad dal and whole wheat flour dosa |</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/quinoa-dosa-41708r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/4 cup urad dal (split black lentils)
-1/2 cup quinoa flour
-1/4 cup whole wheat flour (gehun ka atta)
-salt to taste
-2 1/4 tsp ghee or for cooking
-</t>
-  </si>
-  <si>
-    <t>5 mins</t>
-  </si>
-  <si>
-    <t>25 mins</t>
-  </si>
-  <si>
-    <t>Soak the urad dal in enough water for 1 hour. Drain well.
-Blend in a mixer to a smooth paste using ½ cup of water.
-Combine the remaining ingredients, prepared urad dal paste and ¾ cup of water in a deep bowl, mix well using a whisk.
-Heat a non-stick tava (griddle), sprinkle a little water on the tava (griddle) and wipe it off gently using a cloth.
-Pour a ladleful of the batter on it and spread it in a circular motion to make a 150 mm. (6”) diameter thin circle.
-Smear ¼ tsp oil over it and along the edges and cook on a high flame till the dosa turns brown in colour from both the sides.
-Fold over to make a semi-circle or a roll.
-Repeat with the remaining batter to make 8 more dosas.
-Serve immediately.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy 70 cal
-Protein 2.8 g
-Carbohydrates 10.5 g
-</t>
-  </si>
-  <si>
-    <t>Diabetes</t>
   </si>
 </sst>
 </file>
@@ -132,7 +89,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -173,37 +130,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Added food and recipe categories. Reverted testng settings to parallel processing. Generated new data based on latest input criteria.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/output/SmartScrappers_Team17_Diabetes_To_Add.xlsx
+++ b/src/test/resources/TestData/output/SmartScrappers_Team17_Diabetes_To_Add.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="204">
   <si>
     <t>Recipe ID</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>https://www.tarladalal.com/quinoa-dosa-41708r</t>
+  </si>
+  <si>
+    <t>Breakfast, Snack</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t xml:space="preserve">1/4 cup urad dal (split black lentils)
@@ -140,6 +146,9 @@
   </si>
   <si>
     <t>https://www.tarladalal.com/maharashtrian-patal-bhaji-paatal-bhaji-770r</t>
+  </si>
+  <si>
+    <t>Veg</t>
   </si>
   <si>
     <t xml:space="preserve">2 1/2 cups chopped colocassia leaves (arbi ke patte)
@@ -225,6 +234,9 @@
   </si>
   <si>
     <t>https://www.tarladalal.com/quinoa-veg-upma-vegan-breakfast-42265r</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
   </si>
   <si>
     <t xml:space="preserve">1/2 cup quinoa , washed and drained
@@ -319,6 +331,9 @@
     <t>https://www.tarladalal.com/roasted-capsicum-and-alfalfa-sprouts-salad-with-peanut-dressing-39213r</t>
   </si>
   <si>
+    <t>Jain</t>
+  </si>
+  <si>
     <t xml:space="preserve">2 cups alfalfa sprouts
 1 red capsicum , medium
 1 capsicum , green medium
@@ -391,6 +406,805 @@
 Protein 2.3 g
 Carbohydrates 3.8 g
 </t>
+  </si>
+  <si>
+    <t>42400</t>
+  </si>
+  <si>
+    <t>strawberry steel cut oats with tea masala recipe | steel cut oats with fruits | healthy steel cut oats with chai masala |</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/strawberry-steel-cut-oats-with-tea-masala-42400r</t>
+  </si>
+  <si>
+    <t>Snack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 cup chopped strawberries
+1/2 cup steel cut oats
+1/4 tsp chai ka masala
+1/2 tsp vanilla essence
+1 tsp maple syrup
+1/4 cup chopped strawberries
+1 tbsp roasted sunflower seeds (surajmukhi ke beej)
+</t>
+  </si>
+  <si>
+    <t>For strawberry steel cut oats with tea masala
+To make strawberry steel cut oats with tea masala, soak the steel cut oats in a deep bowl in enough water for 8 hours. Drain well.
+Boil 1 cup of water in a deep non-stick pan, add the soaked and drained oats and mix well. Cover it with a lid and cook on a medium slow flame for 6 minutes, while stirring occasionally. Cool completely.
+Combine the steel cut oats, chai masala, vanilla essence, maple syrup and ½ cup of cold water in a deep bowl and mix well.
+Add the strawberries and mix well.
+Finally top it with the strawberries and sunflower seeds.
+Serve strawberry steel cut oats with tea masala or store in an air-tight container in the fridge and use as required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 219 cal
+Protein 8 g
+Carbohydrates 35.6 g
+</t>
+  </si>
+  <si>
+    <t>42347</t>
+  </si>
+  <si>
+    <t>strawberry oats pudding recipe | healthy oat strawberry pudding | oats strawberry overnight pudding for weight loss | creamy strawberry oats pudding | sugar free pudding |</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/strawberry-oats-pudding-42347r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 cup quick cooking rolled oats
+1/2 cup chopped strawberries
+1 cup almond milk
+</t>
+  </si>
+  <si>
+    <t>For strawberry oats pudding
+To make strawberry oats pudding, combine the oats, strawberry and almond milk in a deep bowl.
+Mix well, cover it with a lid and refrigerate it for overnight.
+Serve the strawberry oats pudding chilled.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 107 cal
+Protein 4 g
+Carbohydrates 16.9 g
+</t>
+  </si>
+  <si>
+    <t>42345</t>
+  </si>
+  <si>
+    <t>Strawberry Almond Milk and Oats Smoothie</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/strawberry-almond-milk-and-oats-smoothie-42345r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 cup frozen chopped strawberries
+1 cup chilled almond milk
+1/2 cup quick cooking rolled oats
+1 tsp maple syrup or honey
+</t>
+  </si>
+  <si>
+    <t>Combine all the ingredients in a mixer and blend it till smooth.
+Pour the smoothie in 2 individual glasses.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 118 cal
+Protein 4 g
+Carbohydrates 19.5 g
+</t>
+  </si>
+  <si>
+    <t>41900</t>
+  </si>
+  <si>
+    <t>lemony quinoa and baby spinach soup recipe | quinoa and dill soup | healthy Indian quinoa baby spinach soup |</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/lemony-quinoa-and-baby-spinach-soup-weight-loss-soup-41900r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 cups vegetable stock
+1/2 cup quinoa
+1 tsp lemon rind
+1 tbsp finely chopped garlic (lehsun)
+1 cup baby spinach , torn into pieces
+1/4 cup chopped dill leaves
+salt and
+1 tbsp lemon juice
+</t>
+  </si>
+  <si>
+    <t>16 mins</t>
+  </si>
+  <si>
+    <t>For lemony quinoa and baby spinach soup
+To make lemony quinoa and baby spinach soup, combine the vegetable stock, quinoa, lemon rind and garlic in a deep non-stick pan, mix well and cook on a medium flame for 15 minutes, while stirring it occasionally.
+Add the spinach, dill, salt and pepper powder and mix well and cook on a medium flame for 1 minute, while it stirring occasionally.
+Switch off the flame add the lemon juice and mix well.
+Serve the lemony quinoa and baby spinach soup immediately.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 115 cal
+Protein 4.5 g
+Carbohydrates 22.4 g
+</t>
+  </si>
+  <si>
+    <t>41520</t>
+  </si>
+  <si>
+    <t>quinoa oats pancakes recipe | quinoa pancakes for Irritable bowel syndrome  | healthy quinoa vegetable Indian pancake |</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/quinoa-oats-pancake-ibs-recipe-41520r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 cup quinoa flour
+1/2 cup oats flour
+1/2 cup grated carrot
+1/2 cup finely chopped spinach (palak)
+1/4 cup grated potatoes
+1/4 tsp finely chopped green chillies
+salt to taste
+1 tsp oil for greasing
+</t>
+  </si>
+  <si>
+    <t>For quinoa oats pancakes
+To make quinoa oats pancakes batter, combine quinoa flour, oats flour, carrots, spinach, potatoes, green chillies and salt along with 1 1/4th cup of water in a deep bowl and mix well.
+Heat a non-stick mini uttapam pan and grease with ¼ tsp of oil. Pour 1 tbsp of the batter into each uttapa mould, spread it evenly.
+Cook on a medium flame for 50 seconds, brush with oil, flip and cook the other side the same way.
+Cook till they turn golden brown in colour from both the sides.
+Repeat to make 1 more batch of quinoa oats vegetable pancakes for irritable bowel syndrome.
+Serve quinoa oats pancakes immediately.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 40 cal
+Protein 1.4 g
+Carbohydrates 6.5 g
+</t>
+  </si>
+  <si>
+    <t>33653</t>
+  </si>
+  <si>
+    <t>Italiano Salad ( Healthy Diabetic Recipe )</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/italiano-salad--healthy-diabetic-recipe--33653r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 tbsp lemon juice
+1 tsp olive oil
+1/4 tsp dried oregano
+1 tsp finely chopped basil leaves
+1 tsp crushed garlic (lehsun)
+1/4 tsp dry red chilli flakes (paprika)
+2 tbsp chopped pine nuts/ walnuts (akhrot)
+salt to taste
+1/2 cup boiled pasta (of your choice)
+1/2 cup bean sprouts
+2 medium tomatoes , deseeded and cubed
+2 medium capsicum , cubed
+3 spring onions (with the greens) , chopped
+5 to 6 stuffed olives , cut into halves
+</t>
+  </si>
+  <si>
+    <t>20 mins</t>
+  </si>
+  <si>
+    <t>Combine all the salad ingredients together in a bowl and mix well. Refrigerate to chill.
+Just before serving, add the dressing and toss well.
+Serve chilled garnished with the olives.
+Disclaimer:
+It is highly recommended that this recipe be relished by diabetics only occasionally and in small quantities. This is just a mere ‘treat’ and does not qualify for a regular diabetic menu.</t>
+  </si>
+  <si>
+    <t>3544</t>
+  </si>
+  <si>
+    <t>jowar vegetable porridge recipe | healthy jowar upma for weight loss | sorghum porridge |</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/jowar-and-vegetable-porridge-3544r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 cup coarsely powdered peanuts
+salt to taste
+1 tsp oil
+1 cup chopped mixed vegetables (french beans ,
+carrot , and cauliflower)
+1/2 tsp mustard seeds ( rai / sarson)
+a pinch of asafoetida (hing)
+2 tbsp finely chopped tomatoes
+2 tbsp finely chopped onions
+2 tbsp finely chopped coriander (dhania)
+</t>
+  </si>
+  <si>
+    <t>For jowar and vegetable porridge
+Combine the powdered jowar, salt with 3 cups of water in a pressure cooker, mix well and pressure cook for 4 whistles.
+Allow the steam to escape before opening the lid.
+Heat the oil in a deep pan and add the mustard seeds and asafoetida.
+When the mustard seeds crackle, add the mixed vegetables and sauté on a medium flame for 3 to 4 minutes.
+Add the cooked jowar mixture, 1½ cups of water and salt, mix well and simmer for 8 to 10 minutes, while stirring occasionally.
+Top with the tomato, onion and coriander and serve immediately.
+Handy tips
+To get ½ cup of coarsely ground jowar, grind ½ cup of jowar in a mixer to a coarse powder.
+If the porridge becomes too thick while serving, adjust its consistency by some adding some water.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 103 cal
+Protein 3.3 g
+Carbohydrates 18.6 g
+</t>
+  </si>
+  <si>
+    <t>33763</t>
+  </si>
+  <si>
+    <t>Green Papaya Salad ( Exotic Diabetic Recipe )</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/green-papaya-salad--exotic-diabetic-recipe--33763r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 tsp crushed green chillies
+2 tsp sugar substitute
+1 tsp tamarind (imli) pulp
+1 tsp chilli powder
+2 tsp soy sauce
+2 tsp lemon juice
+2 tbsp chopped coriander (dhania)
+salt to taste
+3 cups grated raw papaya
+3/4 cup thinly sliced tomatoes
+1/4 cup peanuts , roasted and powdered
+</t>
+  </si>
+  <si>
+    <t>Combine the green chillies, sugar substitute, tamarind pulp, chilli powder, soya sauce, lemon juice, coriander and salt together and pound using a mortar-pestle (khalbhatta) and to a coarse paste. Keep aside.
+Put the raw papaya in ice-cold water for half an hour. This will make it crisp.
+Drain, wrap in a muslin cloth and refrigerate till ready to use.
+Combine all the ingredients together in a serving bowl and toss well.
+Serve immediately.
+Disclaimer:
+It is highly recommended that this recipe be relished by diabetics only occasionally and in small quantities. This is just a mere ‘treat’ and does not qualify for a regular diabetic menu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 61 cal
+Protein 2.6 g
+Carbohydrates 7.7 g
+</t>
+  </si>
+  <si>
+    <t>36898</t>
+  </si>
+  <si>
+    <t>Date and Apple Kheer</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/date-and-apple-kheer-36898r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 cup chopped apples
+1 tsp sugar
+2 1/2 cups low fat milk
+2 sachets sugar substitute (1 gm each)
+1/4 cup chopped dates (khajur)
+1 tbsp chopped walnuts (akhrot)
+1 tbsp finely chopped apples
+</t>
+  </si>
+  <si>
+    <t>Combine the apples, sugar and 3 tbsp of water in a non-stick pan and cook over a medium flame for 2 to 3 minutes, while stirring continuously. Refrigerate to chill.
+Combine the milk, sugar substitute and dates in a deep non-stick pan, mix well and simmer for 10 minutes while stirring continuously. Refrigerate to chill.
+Just before serving add the cooked apples to the milk-dates mixture and mix gently.
+Serve chilled garnished with walnuts and apples.
+Disclaimer:
+It is highly recommended that this recipe be relished by diabetics only occasionally and in small quantities. This is just a mere ‘treat’ and does not qualify for a regular diabetic menu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 77 cal
+Protein 4.5 g
+Carbohydrates 14.1 g
+</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>kaddu ka raita recipe | red pumpkin raita | healthy kaddu ka raita |</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/kaddu-ka-raita-1994r</t>
+  </si>
+  <si>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 cups finely chopped red pumpkin (bhopla / kaddu)
+1 tsp ghee
+1 tsp cumin seeds (jeera)
+2 tsp finely chopped green chillies
+1 tsp sugar (optional)
+1 1/2 cups whisked curds (dahi)
+2 tbsp milk
+salt to taste
+1 tbsp crushed roasted peanuts
+2 tsp finely chopped coriander (dhania)
+</t>
+  </si>
+  <si>
+    <t>7 mins</t>
+  </si>
+  <si>
+    <t>For kaddu ka raita
+To make kaddu ka raita, heat the ghee in a deep pan and add the cumin seeds.
+When the seeds crackle, add the pumpkin, salt and sugar, mix well and cover and cook on a medium flame for 6 minutes, while stirring occasionally.
+Add the green chillies and sauté on a medium flame for a few seconds.
+Remove from the flame and allow it to cool for 2 minutes.
+Once cooled, mash the pumpkin pieces with help of a masher.
+Add the curds and mix well.
+Refrigerate the kaddu ka raita for 1 hour and serve chilled garnished with peanuts and coriander.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 134 cal
+Protein 4.8 g
+Carbohydrates 9.3 g
+</t>
+  </si>
+  <si>
+    <t>22197</t>
+  </si>
+  <si>
+    <t>Mushroom and Green Peas Curry</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/mushroom-and-green-peas-curry-22197r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 tbsp chopped cashewnuts (kaju)
+2 tbsp poppy seeds (khus-khus) , soaked in 2 tablespoons of water
+2 green chillies , roughly chopped
+2 cloves (laung / lavang)
+2 garlic (lehsun) cloves
+2 cardamoms (elaichi)
+1 tsp chopped ginger (adrak)
+1/2 cup chopped onions
+2 cups vegetable stock
+1 cup green peas
+salt to taste
+1 1/2 cups sliced mushrooms (khumbh)
+1/4 cup fresh low fat curds (dahi)
+1/4 cup low fat milk
+2 tbsp chopped coriander (dhania) for garnishing
+</t>
+  </si>
+  <si>
+    <t>Heat a non-stick pan on a medium flame and when hot, add the ground paste.
+Cook while stirring continuously till it is light brown in colour. Sprinkle a little water if the paste burns.
+Add the onions and dry roast while stirring continuously till they turn translucent.
+Add ½ cup of vegetable stock to it and mix well till smooth. Keep aside.
+Heat a non-stick kadhai on a medium flame and when hot, add the peas, salt and the remaining vegetable stock.
+When it starts boiling, add the ground paste and simmer till the peas get cooked.
+Add the mushrooms, curds and milk and simmer for another 5 minutes.
+Serve hot garnished with coriander.</t>
+  </si>
+  <si>
+    <t>22171</t>
+  </si>
+  <si>
+    <t>Toovar Dal with Vegetables</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/toovar-dal-with-vegetables-22171r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/4 cup toovar (arhar) dal , soaked for 2 hours and drained
+salt to taste
+1/2 tsp turmeric powder (haldi)
+1/4 cup yam (suran) cubes
+1 tbsp raw peanuts
+2 drumsticks , cut into 50 mm. (2") pieces
+5 to 6 curry leaves (kadi patta)
+1 tbsp grated jaggery (gur)
+1 tbsp tamarind (imli) pulp
+1 tsp ginger-green chilli paste
+1 tbsp finely chopped coriander (dhania)
+1/4 cup ladies finger (bhindi) (with edges trimmed)
+rice
+parathas
+</t>
+  </si>
+  <si>
+    <t>Combine the toovar dal, 1 cup of water, salt, turmeric powder, yam, peanuts and drumsticks, mix well and pressure cook for 2 whistles.
+Allow the steam to escape before opening the lid.
+Add 1 cup of water, mix well and mash with the back of a spoon.
+Add the curry leaves, jaggery, tamarind pulp, ginger-green chilli paste, coriander and ladies finger, mix well and cook on a slow flame for 5 to 7 minutes, while stirring occasionally.
+Serve hot with rice and parathas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 78 cal
+Protein 3.4 g
+Carbohydrates 12.7 g
+</t>
+  </si>
+  <si>
+    <t>33764</t>
+  </si>
+  <si>
+    <t>Lettuce Wraps ( Exotic Diabetic Recipe )</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/lettuce-wraps--exotic-diabetic-recipe--33764r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 tsp oil
+2 tsp finely chopped garlic (lehsun)
+1 tsp finely chopped galangal (thai ginger)
+1/4 cup chopped spring onions with the greens
+1/4 cup chopped mushrooms (khumbh)
+1/4 cup finely chopped carrots
+1/4 cup finely chopped cabbage
+1/4 cup chopped bean sprouts
+1/4 cup chopped tofu (bean curd/soya paneer)
+1/2 tsp lemon juice
+1 tsp soy sauce
+salt to taste
+1/4 tsp dry red chilli flakes (paprika)
+6 lettuce leaves
+2 tbsp peanuts , roasted and coarsely ground
+2 tbsp finely chopped fresh basil leaves
+</t>
+  </si>
+  <si>
+    <t>For the stuffing
+Heat the oil in a non-stick kadhai, add the garlic, ginger and spring onions and sauté till the onions turn translucent.
+Add the mushrooms, carrots and cabbage, mix well and sauté on a medium flame for 2 to 3 minutes.
+Add the bean sprouts, tofu, lemon juice, soya sauce, salt and red chilli flakes, mix gently and saute on a medium flame for another minute.
+Divide the stuffing into 6 equal portions and keep aside.
+How to proceed
+Wash the lettuce leaves, dry them on a towel and keep aside.
+Place a lettuce leaf on a clean, flat surface and place a portion of the stuffing along one side of the leaf.
+Add ½ tsp of peanuts and ½ tsp of basil over the stuffing, roll it up gently and secure the roll by inserting a toothpick or tie using a spring onion green.
+Repeat with the remaining ingredients to make 5 more wraps.
+Serve immediately.
+Disclaimer:
+It is highly recommended that this recipe be relished by diabetics only occasionally and in small quantities. This is just a mere ‘treat’ and does not qualify for a regular diabetic menu.</t>
+  </si>
+  <si>
+    <t>33765</t>
+  </si>
+  <si>
+    <t>Thai Pineapple Kodri ( Exotic Diabetic Recipe )</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/thai-pineapple-kodri--exotic-diabetic-recipe--33765r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 stalks lemon grass (harechai ki patti) , finely chopped
+1 tbsp roasted cumin seeds (jeera)
+1 tbsp roasted coriander (dhania) seeds
+1/2 tbsp grated ginger (adrak)
+2 whole dry kashmiri red chillies , deseeded
+2 garlic (lehsun) cloves
+1/2 small onion , quartered
+1/2 tsp turmeric powder (haldi)
+salt to taste
+2 tsp oil
+1/2 cup chopped onions
+1 tsp finely chopped green chillies
+2 cups finely chopped fresh pineapple
+1/4 cup coconut milk
+2 tsp chopped raisins (kismis)
+1 tsp sugar substitute
+salt to taste
+2 1/2 cups cooked kodri (varagu)
+4 lemon slices
+2 cashewnuts (kaju) , cut into halves
+</t>
+  </si>
+  <si>
+    <t>Heat the oil in a non-stick kadhai, add the onions and green chillies and sauté on a medium flame till the onions turn translucent.
+Add the yellow curry paste and sauté for a minute.
+Add the pineapple, coconut milk, raisins, sugar substitute and salt, mix well and cook over a medium flame for 8 to 10 minutes, while gently stirring continuously.
+Add the kodri, mix gently and cook for another minute.
+Serve hot garnished with lemon slices and cashewnuts.
+Disclaimer:
+It is highly recommended that this recipe be relished by diabetics only occasionally and in small quantities. This is just a mere ‘treat’ and does not qualify for a regular diabetic menu.</t>
+  </si>
+  <si>
+    <t>33766</t>
+  </si>
+  <si>
+    <t>Phadthai Noodles ( Exotic Diabetic Recipe )</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/phadthai-noodles--exotic-diabetic-recipe--33766r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 tsp oil
+2 tsp finely chopped garlic (lehsun)
+1/2 cup tofu cubes
+1/2 cup chopped spring onions with the greens
+1 cup bean sprouts
+2 tbsp roasted and coarsely powdered peanuts
+3 cups cooked noodles , refer handy tip
+3/4 tsp dry red chilli flakes (paprika)
+1 tsp sugar substitute
+1 tsp soy sauce
+1 tbsp lemon juice
+salt to taste
+2 tbsp chopped coriander (dhania)
+</t>
+  </si>
+  <si>
+    <t>Heat the oil in a deep non-stick pan, add the garlic and sauté over a high flame for a minute, while stirring continuously.
+Add the all the remaining ingredients and toss well and cook on a medium flame for another minute.
+Serve hot garnished with coriander.
+Handy tip:
+To cook 3 cups of rice noodles, soak 3/4 packet of raw rice noodles in boiling hot water for 10 to 15 minutes or as the instructions on the package specify. Drain the water and immerse in cold water in order to arrest any further cooking. Drain and use as required.
+This recipe has been developed only to satisfy the occasionally craving of a diabetic for exotic dishes as it contains certain ingredients which need to be used restrictively. Hence this does not qualify as a regular everyday meal.
+Disclaimer:
+It is highly recommended that this recipe be relished by diabetics only occasionally and in small quantities. This is just a mere ‘treat’ and does not qualify for a regular diabetic menu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 179 calories
+Protein 9.3 gm
+Carbohydrates 20.5 gm
+</t>
+  </si>
+  <si>
+    <t>33789</t>
+  </si>
+  <si>
+    <t>Walnut Vegetable Paté with Toasted Triangles ( Diabetic Recipe )</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/walnut-vegetable-pat%C3%A9-with-toasted-triangles--diabetic-recipe--33789r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 tsp olive oil
+3/4 cup finely chopped mixed vegetables (mushrooms , spring onions , carrot , etc.)
+1/4 cup chopped walnuts (akhrot)
+1 tsp chopped garlic (lehsun)
+1/2 tsp dried mixed herbs
+salt to taste
+8 toasted whole wheat bread , cut into triangles
+tabasco sauce
+a few lettuce leaves , torn into pieces
+4 cherry tomatoes , cut into halves
+</t>
+  </si>
+  <si>
+    <t>Heat the oil in a non-stick pan, add the mixed vegetables and sauté over a medium flame for 2 minutes.
+Remove from the flame, add the walnuts, garlic, mixed dried herbs and salt and blend in a mixer with a little water to get a grainy purée.
+For serving. Place a small lettuce leaf on each toasted triangle,spread little paté on each toasted triangle, top with few drops of tabasco sauce.
+Garnish with cherry tomatoes and serve immediately.
+Disclaimer:
+It is highly recommended that this recipe be relished by diabetics only occasionally and in small quantities. This is just a mere ‘treat’ and does not qualify for a regular diabetic menu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 89 cal
+Protein 2 g
+Carbohydrates 3 g
+</t>
+  </si>
+  <si>
+    <t>33704</t>
+  </si>
+  <si>
+    <t>Sugar Free Date Rolls, Healthy Diabetic Recipe</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/sugar-free-date-rolls-healthy-diabetic-recipe-33704r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 tsp ghee
+3/4 cup deseeded and finely chopped black dates (kala khajur)
+1 tbsp chopped almonds (badam)
+1 tbsp chopped pistachios
+1 tbsp chopped walnuts (akhrot)
+2 tbsp poppy seeds (khus-khus) for coating
+</t>
+  </si>
+  <si>
+    <t>Heat the ghee in a small non-stick pan, add the dates and cook on a slow flame, while stirring continuously for 5 to 7 minutes or till they turn into a soft lump.
+Remove and add the almonds, pistachio nuts and walnuts and mix well.
+Divide into 6 equal portions and shape each portion into a roll.
+Coat each roll with poppy seeds and refrigerate to set.
+Disclaimer:
+It is highly recommended that this recipe be relished by diabetics only occasionally and in small quantities. This is just a mere ‘treat’ and does not qualify for a regular diabetic menu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 79 cal
+Protein 1.6 g
+Carbohydrates 7.1 g
+</t>
+  </si>
+  <si>
+    <t>43053</t>
+  </si>
+  <si>
+    <t>bajra churma ladoo recipe | leftover bajra roti ladoo | quick bajra ladoo recipe |</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/bajra-churma-ladoo-43053r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 cup bajra (black millet) flour
+2 tbsp roasted chopped mixed nuts
+2 tbsp roasted sesame seeds (til)
+2 tsp ghee
+2 tbsp chopped jaggery (gur)
+</t>
+  </si>
+  <si>
+    <t>2 mins</t>
+  </si>
+  <si>
+    <t>For bajra churma ladoo
+To make bajra churma ladoo, heat ghee in a small pan, add the jaggery and 4 tbsp water and mix well.
+Cook on medium flame for 3 to 4 minutes until the jaggery melts completely. Keep aside.
+In a deep bowl combine the bajra flour along with 1/3 cup of water and knead into a soft dough.
+Divide the dough into 2 equal portions and roll each portion into a 150 mm. (6”) diameter roti using little bajra flour for patting.
+Heat a non-stick tava (griddle), place the roti over it and apply little water evenly.
+Cook it for a few seconds, turn over the roti, and cook the other side for a few more seconds.
+Lift the roti with a pair of flat tongs and roast over an open flame till brown spots appear on both sides.
+Repeat steps 2 to 5 to make 1 more bajra roti.
+Remove in a plate and allow it to cool completely.
+Once cooled break into pieces and blend it to make a coarse mixture.
+Transfer the mixture into a deep bowl, add mixed nuts, sesame seeds, and the prepared jaggery syrup.
+Mix well until well with your hands.
+Divide the mixture into 10 equal portions and shape each portion into a round ladoo.
+Serve the bajra churma ladoo or store in an air-tight container. They stay fresh for a day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 69 cal
+Protein 1.5 g
+Carbohydrates 10.4 g
+</t>
+  </si>
+  <si>
+    <t>43061</t>
+  </si>
+  <si>
+    <t>healthy parfait recipe | Indian style yoghurt parfait | diabetes friendly fruit and yogurt parfait |</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/healthy-indian-parfait-43061r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/4 cup rolled oats
+3 tbsp roasted mixed chopped nuts
+1 tbsp roasted pumpkin seeds
+1 tbsp roasted sunflower seeds (surajmukhi ke beej)
+1 tbsp chopped raisins (kismis)
+sea salt (khada namak) to taste
+1 cup hung low fat curds (chakka dahi)
+1/2 tsp vanilla extract
+1/4 cup chopped apple
+1/4 cup chopped pears
+1/4 cup pomegranate seeds (anardana)
+</t>
+  </si>
+  <si>
+    <t>3 mins</t>
+  </si>
+  <si>
+    <t>For healthy parfait
+To make healthy parfait, dry roast oats in a non-stick pan on medium flame for 2 to 3 minutes.
+Remove in a bowl and cool completely. Add roasted mixed nuts, pumpkin seeds, sunflower seeds, chopped raisin and sea salt to taste. Mix well and keep aside.
+Combine hung curd and vanilla extract in a deep bowl, whisk well and keep aside.
+Take a serving glass, put 2 tbsp of granola, 2 tbsp hung curd mixture and 1 tbsp mixed fruit mixture.
+Repeat step 4 to make one more parfait layer.
+Repeat step 4 and 5 to make 1 more glass of parfait.
+Serve the healthy parfait immediately.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 179 cal
+Protein 10.3 g
+Carbohydrates 26 g
+</t>
+  </si>
+  <si>
+    <t>43076</t>
+  </si>
+  <si>
+    <t>quinoa khichdi recipe | healthy quinoa khichdi | instant pot quinoa khichdi |</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/quinoa-khichdi-43076r</t>
+  </si>
+  <si>
+    <t>Vegetarian, Veg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 cup quinoa , washed and drained
+1/2 cup yellow moong dal (split yellow gram)
+2 tsp ghee
+1 cinnamon (dalchini) stick
+2 tsp mustard seeds ( rai / sarson)
+1/2 tbsp crushed panch phoron
+2 tsp chopped pandi chillies
+8 to 10 curry leaves (kadi patta)
+a pinch of asafoetida (hing)
+1/2 cup finely chopped onions
+1/2 tbsp ginger-garlic (adrak-lehsun) paste
+1 tsp green chilli paste
+1/4 cup finely chopped tomatoes
+1 cup blanched and chopped mixed vegetables
+1/2 tsp turmeric powder (haldi)
+1/2 tsp chilli powder
+1/4 tsp garam masala
+salt to taste
+1 tsp lemon juice
+2 tbsp finely chopped coriander (dhania)
+</t>
+  </si>
+  <si>
+    <t>30 mins</t>
+  </si>
+  <si>
+    <t>For masala quinoa khichdi
+To make masala quinoa khichdi recipe, combine quinoa, yellow moong, 3 cups of water and salt to taste in a pressure cooker.
+Pressure cook it for 2 whistles. Allow the steam to escape and then open the lid. Mix well and keep aside.
+Heat ghee in a deep pan, add cinnamon, mustard, panch phoron, dry red chillies, curry leaves and asafetida, sauté for few seconds.
+Add onions and sauté on medium flame for 2 minutes, add ginger garlic paste, green chilli paste and sauté for a few seconds.
+Add tomatoes and sauté on medium flame for 2 minutes, while stirring occasionally.
+Add the mixed chopped vegetables, turmeric powder, chilli powder and garam masala.
+Mix well and cook on medium flame for 2 minutes, while stirring occasionally.
+Add the cooked quinoa-dal mixture, 1 cup hot water, salt to taste and mix well and cook on medium flame for 4 to 5 minutes.
+Switch off the flame and add the lemon juice and coriander, mix well.
+Serve masala quinoa khichdi hot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy 150 cal
+Protein 7.3 g
+Carbohydrates 25 g
+</t>
+  </si>
+  <si>
+    <t>36200</t>
+  </si>
+  <si>
+    <t>Pumpkin Pulao</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/pumpkin-pulao-36200r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 cup cooked long grained rice
+1/2 cup roasted and chopped pumpkin
+1/4 cup roasted and chopped red capsicum
+1/2 cup chopped fenugreek (methi) leaves
+1/4 cup roasted and crushed peanuts
+1 tbsp ghee
+2 tsp cumin seeds (jeera)
+2 bayleaf (tejpatta)
+1 star anise (chakri phool)
+salt to taste
+1 tsp sugar
+1 tsp chopped green chillies
+2 tsp grated ginger (adrak)
+1 few curry leaves (kadi patta)
+2 tbsp rose water
+</t>
+  </si>
+  <si>
+    <t>Heat ghee in deep non stick kadhai and add the cumin seeds.
+When the seeds crackle, add the bay leaf and star anise and saute for 10 seconds.
+Add the ginger, green chillies and curry leaves and saute for more 10 seconds.
+Add the pumpkin, capsicum, fenugreek leaves and sugar and mix well.
+Add the cooked rice, salt, rose water and peanuts, mix well and saute for 5 minutes.
+Serve hot.</t>
   </si>
 </sst>
 </file>
@@ -435,7 +1249,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -486,242 +1300,1009 @@
       <c r="C2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
+      <c r="D2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>15</v>
+      </c>
       <c r="F2" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
+        <v>24</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>15</v>
+      </c>
       <c r="F3" t="s" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="D4" s="0"/>
-      <c r="E4" s="0"/>
+        <v>32</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>33</v>
+      </c>
       <c r="F4" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="D5" s="0"/>
-      <c r="E5" s="0"/>
+        <v>40</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>15</v>
+      </c>
       <c r="F5" t="s" s="0">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="D6" s="0"/>
-      <c r="E6" s="0"/>
+        <v>47</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>15</v>
+      </c>
       <c r="F6" t="s" s="0">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
+        <v>55</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>33</v>
+      </c>
       <c r="F7" t="s" s="0">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="G8" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="C8" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>53</v>
-      </c>
       <c r="H8" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="K8" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
+        <v>69</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>15</v>
+      </c>
       <c r="F9" t="s" s="0">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="J9" t="s" s="0">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="K9" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="K10" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="K11" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="K12" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="K13" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="G14" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H14" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I14" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="J14" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="K14" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="H15" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="I15" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="J15" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="G16" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="H16" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I16" t="s" s="0">
+        <v>116</v>
+      </c>
+      <c r="J16" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="K16" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>120</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="G17" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="H17" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="I17" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="J17" t="s" s="0">
+        <v>123</v>
+      </c>
+      <c r="K17" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>127</v>
+      </c>
+      <c r="G18" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H18" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="I18" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="J18" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="K18" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>130</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>131</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>132</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="G19" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H19" t="s" s="0">
+        <v>135</v>
+      </c>
+      <c r="I19" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="J19" t="s" s="0">
+        <v>137</v>
+      </c>
+      <c r="K19" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>140</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="G20" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="H20" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="I20" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J20" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="K20" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>145</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="G21" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H21" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="I21" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="J21" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="K21" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>151</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="G22" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H22" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="I22" t="s" s="0">
+        <v>153</v>
+      </c>
+      <c r="J22" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="K22" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>154</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>155</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>156</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s" s="0">
+        <v>157</v>
+      </c>
+      <c r="G23" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H23" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="I23" t="s" s="0">
+        <v>158</v>
+      </c>
+      <c r="J23" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="K23" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>159</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>161</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="G24" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H24" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I24" t="s" s="0">
+        <v>163</v>
+      </c>
+      <c r="J24" t="s" s="0">
+        <v>164</v>
+      </c>
+      <c r="K24" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>167</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="G25" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H25" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I25" t="s" s="0">
+        <v>169</v>
+      </c>
+      <c r="J25" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="K25" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>173</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="G26" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="H26" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="I26" t="s" s="0">
+        <v>175</v>
+      </c>
+      <c r="J26" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="K26" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>177</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>178</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>179</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s" s="0">
+        <v>180</v>
+      </c>
+      <c r="G27" t="s" s="0">
+        <v>181</v>
+      </c>
+      <c r="H27" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I27" t="s" s="0">
+        <v>182</v>
+      </c>
+      <c r="J27" t="s" s="0">
+        <v>183</v>
+      </c>
+      <c r="K27" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>184</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>185</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>186</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s" s="0">
+        <v>187</v>
+      </c>
+      <c r="G28" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H28" t="s" s="0">
+        <v>188</v>
+      </c>
+      <c r="I28" t="s" s="0">
+        <v>189</v>
+      </c>
+      <c r="J28" t="s" s="0">
+        <v>190</v>
+      </c>
+      <c r="K28" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="F29" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="G29" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="H29" t="s" s="0">
+        <v>196</v>
+      </c>
+      <c r="I29" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="J29" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="K29" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>200</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>201</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="F30" t="s" s="0">
+        <v>202</v>
+      </c>
+      <c r="G30" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H30" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="I30" t="s" s="0">
+        <v>203</v>
+      </c>
+      <c r="J30" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="K30" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>